<commit_message>
revised microhabitat1 vector back to match version 10.
</commit_message>
<xml_diff>
--- a/data/Carrizo_telemetry_2018_10.xlsx
+++ b/data/Carrizo_telemetry_2018_10.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25280" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -963,7 +963,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -973,9 +973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1245"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M985" sqref="A1:S1245"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <sheetData>

</xml_diff>